<commit_message>
Live Project in POM Framework
</commit_message>
<xml_diff>
--- a/SeleniumPOMFramework/TestData/RediffPortFolioLaunch.xlsx
+++ b/SeleniumPOMFramework/TestData/RediffPortFolioLaunch.xlsx
@@ -9,13 +9,14 @@
   </bookViews>
   <sheets>
     <sheet name="RediffLoginTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="StockTestData" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>openPorfolio</t>
   </si>
@@ -63,6 +64,48 @@
   </si>
   <si>
     <t>Invalid Credentials</t>
+  </si>
+  <si>
+    <t>addPortfolioTest</t>
+  </si>
+  <si>
+    <t>PortfolioName</t>
+  </si>
+  <si>
+    <t>SME Stocks</t>
+  </si>
+  <si>
+    <t>SME Stock Portfolio</t>
+  </si>
+  <si>
+    <t>HighGain Stocks</t>
+  </si>
+  <si>
+    <t>HighGain Stocks Portfolio</t>
+  </si>
+  <si>
+    <t>BSE Stocks</t>
+  </si>
+  <si>
+    <t>BSE Stocks Portfolio</t>
+  </si>
+  <si>
+    <t>AddStockTest</t>
+  </si>
+  <si>
+    <t>StockName</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>StockPrice</t>
+  </si>
+  <si>
+    <t>My 2019 Stocks</t>
+  </si>
+  <si>
+    <t>Bosch Ltd</t>
   </si>
 </sst>
 </file>
@@ -182,7 +225,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -190,7 +233,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.7"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9030612244898"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.4285714285714"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1275510204082"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.3979591836735"/>
@@ -289,6 +333,43 @@
       </c>
       <c r="D11" s="0" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -306,4 +387,68 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.7"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="14.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>